<commit_message>
Made changes to Create_data.sah and new_sheet
Made changes to Create_data.sah and new_sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/new_sheet.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/new_sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="7260" windowWidth="28160" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Account</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Component</t>
   </si>
   <si>
-    <t>OrderStatus</t>
-  </si>
-  <si>
     <t>ClosedOn</t>
   </si>
   <si>
@@ -102,13 +99,64 @@
   </si>
   <si>
     <t>user_meghana</t>
+  </si>
+  <si>
+    <t>System.Today()</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Case case_1 = new Case (Status = 'Closed' );insert case_1 ;</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Open' );insert SR_1 ;</t>
+  </si>
+  <si>
+    <t>2017-12-21 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-12-21 13:00:00</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>2017-12-10 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-12-10 16:00:00</t>
+  </si>
+  <si>
+    <t>meghana.rao@servicemax.com</t>
+  </si>
+  <si>
+    <t>cloud_101</t>
+  </si>
+  <si>
+    <t>005q0000003GGfP</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed', SVMXC__Priority__c = 'High' );insert SR_1 ;</t>
+  </si>
+  <si>
+    <t>Parts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +180,37 @@
       <sz val="11"/>
       <color rgb="FF3933FF"/>
       <name val="Monaco"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,10 +230,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -167,8 +248,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,13 +540,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="25.1640625" customWidth="1"/>
+    <col min="18" max="18" width="32.6640625" customWidth="1"/>
+    <col min="19" max="19" width="40" customWidth="1"/>
+    <col min="25" max="25" width="37.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -466,70 +569,188 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:25" ht="192" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>43121</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44640</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1">
+        <v>360</v>
+      </c>
+      <c r="X2" s="3">
+        <v>98.33</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="240" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>